<commit_message>
Build site at 2022-10-20 19:00:34 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -393,12 +393,62 @@
         <t xml:space="preserve">Updated on 26-Sep-2022 06:24 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT21">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 04:39 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU21">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 04:39 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV21">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 04:40 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW21">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 04:39 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX21">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 04:39 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DT22">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU22">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV22">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW22">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX22">
+      <text>
+        <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="623">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2099,19 +2149,128 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnucbj-Z5lGg5zqSUeC0uGNS6x3UHr7c6QKiUefEPKxxxosa7GqcU3vKdHBkmu8faUMw&amp;source=documentstudio&amp;timestamp=1664227429679</t>
   </si>
   <si>
+    <t>Daniel Alexandre da Costa Ximenes</t>
+  </si>
+  <si>
+    <t>danielacximenes@gmail.com</t>
+  </si>
+  <si>
+    <t>Barra do Piraí</t>
+  </si>
+  <si>
+    <t>Rua São João n 657</t>
+  </si>
+  <si>
+    <t>São João</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFF - Universidade Federal Fluminense </t>
+  </si>
+  <si>
+    <t>UFF - Universidade Federal Fluminense</t>
+  </si>
+  <si>
+    <t>Engenharia Metalúrgica</t>
+  </si>
+  <si>
+    <t>BTG - Pactual</t>
+  </si>
+  <si>
+    <t>Analista de Investimento</t>
+  </si>
+  <si>
+    <t>CSN - Companhia Siderúrgica Nacional</t>
+  </si>
+  <si>
+    <t>Engenheiro de desenvolvimento de produtos</t>
+  </si>
+  <si>
+    <t>Gerente de Inovação e Tecnologia</t>
+  </si>
+  <si>
+    <t>Além do alto nível de aprendizado durante a realização das matérias, a expectativa é elevar de forma significativa o conhecimento técnico de materiais em aço de forma a buscar a produção de um aço que hoje é uma demanda de mercado assim como uma lacuna técnica e tecnológica.</t>
+  </si>
+  <si>
+    <t>DESENVOLVIMENTO DE UM AÇO PARA ESTAMPAGEM A QUENTE SEM REVESTIMENTO RESISTENTE À OXIDAÇÃO</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1DsS96LIxgPg4NGhgIiXWQag6jRXyt9El</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1BI90pQ7LK430tsztWn8CExKTHuXvue_1</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=139peeg-yVh2UcE7bEgtPMCpoiUGmpKf3</t>
+  </si>
+  <si>
+    <t>2_ABaOnud9LLagnUaTdk0gs8eOY-_s1gsfBdNr0DtM6E5euCAo-KWjHJkPi5MEhc9H6kNL018</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnud9LLagnUaTdk0gs8eOY-_s1gsfBdNr0DtM6E5euCAo-KWjHJkPi5MEhc9H6kNL018&amp;source=documentstudio&amp;timestamp=1666208361148</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro / Brasil</t>
+  </si>
+  <si>
+    <t>Rua São João n657  Ap603</t>
+  </si>
+  <si>
+    <t>Mariana Fialho Ximenes</t>
+  </si>
+  <si>
+    <t>Rua São João n657 ap603</t>
+  </si>
+  <si>
+    <t>Analista de Investimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSN - Companhia Siderúrgica Nacional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Além do alto nível de aprendizado durante a realização das matérias, a expectativa é elevar de forma significativa o conhecimento técnico de materiais em aço de forma a buscar a produção de um aço que hoje é uma demanda de mercado assim como uma lacuna técnica e tecnológica.
+</t>
+  </si>
+  <si>
+    <t>DESENVOLVIMENTO DE UM AÇO PARA ESTAMPAGEM A QUENTE SEM  REVESTIMENTO RESISTENTE À OXIDAÇÃO</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1X_fWnhNxm0EWjhUdYzJvxa00jCDAg9B2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1LYNZfHZQtK6_dLfL04N5ifds6wRP4liD</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1g6I2M1sVqCo3TwlnJ67zQPrjum4S8IYZ</t>
+  </si>
+  <si>
+    <t>2_ABaOnue9bYR30NiS5xhgj_0cGTLQCas0WK2AiqdNcGtwRoEkyFP5N_e_c110Pz35FCXg9qQ</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnue9bYR30NiS5xhgj_0cGTLQCas0WK2AiqdNcGtwRoEkyFP5N_e_c110Pz35FCXg9qQ&amp;source=documentstudio&amp;timestamp=1666209668734</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
   </si>
   <si>
+    <t>✔️  [Respostas] Processed form row #22 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #21 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>⚠️  Google Form has duplicate question titles</t>
+  </si>
+  <si>
+    <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')</t>
+  </si>
+  <si>
     <t>✔️  [Respostas] Processed form row #20 by luizeleno@usp.br</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #19 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>⚠️  Google Form has duplicate question titles</t>
   </si>
   <si>
     <t>inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
@@ -7383,6 +7542,500 @@
         <v>565</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="6">
+        <v>44853.69399476852</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I21" s="7">
+        <v>44925.0</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.2506500771E11</v>
+      </c>
+      <c r="M21" s="2">
+        <v>2.23002262E8</v>
+      </c>
+      <c r="N21" s="7">
+        <v>43712.0</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1.1582689E7</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T21" s="2">
+        <v>2.725336E7</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V21" s="2">
+        <v>2.4999317271E10</v>
+      </c>
+      <c r="W21" s="2">
+        <v>2.4999317272E10</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>2.725336E7</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>2.499931727E10</v>
+      </c>
+      <c r="AE21" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="AF21" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AG21" s="7">
+        <v>41275.0</v>
+      </c>
+      <c r="AH21" s="7">
+        <v>43452.0</v>
+      </c>
+      <c r="AI21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="AK21" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="AL21" s="7">
+        <v>39234.0</v>
+      </c>
+      <c r="AM21" s="7">
+        <v>41426.0</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR21" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="BS21" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="BT21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU21" s="7">
+        <v>41306.0</v>
+      </c>
+      <c r="BV21" s="7">
+        <v>41491.0</v>
+      </c>
+      <c r="BW21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX21" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="BY21" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="BZ21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA21" s="7">
+        <v>41505.0</v>
+      </c>
+      <c r="CB21" s="7">
+        <v>44105.0</v>
+      </c>
+      <c r="CC21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CD21" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="CE21" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="CF21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CG21" s="7">
+        <v>44105.0</v>
+      </c>
+      <c r="CI21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DL21" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="DM21" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN21" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="DO21" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="DP21" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="DT21" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="DU21" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=139peeg-yVh2UcE7bEgtPMCpoiUGmpKf3","Inscrição DOUTORADO PPGEM EEL-USP - Daniel Alexandre da Costa Ximenes.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Daniel Alexandre da Costa Ximenes.pdf</v>
+      </c>
+      <c r="DV21" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/183f1c2868721435","Email sent to ppgem-eel@usp.br, danielacximenes@gmail.com")</f>
+        <v>Email sent to ppgem-eel@usp.br, danielacximenes@gmail.com</v>
+      </c>
+      <c r="DW21" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="DX21" s="9" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6">
+        <v>44853.70912886574</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I22" s="7">
+        <v>32507.0</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.250650771E10</v>
+      </c>
+      <c r="M22" s="2">
+        <v>2.23002262E8</v>
+      </c>
+      <c r="N22" s="7">
+        <v>43712.0</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1.1582689E7</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T22" s="2">
+        <v>2.725336E7</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V22" s="2">
+        <v>2.4999317271E10</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>2.725336E7</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>2.499931727E10</v>
+      </c>
+      <c r="AE22" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AG22" s="7">
+        <v>41275.0</v>
+      </c>
+      <c r="AH22" s="7">
+        <v>41626.0</v>
+      </c>
+      <c r="AI22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="AK22" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="AL22" s="7">
+        <v>39234.0</v>
+      </c>
+      <c r="AM22" s="7">
+        <v>41255.0</v>
+      </c>
+      <c r="AN22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR22" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="BS22" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="BT22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU22" s="7">
+        <v>41306.0</v>
+      </c>
+      <c r="BV22" s="7">
+        <v>41491.0</v>
+      </c>
+      <c r="BW22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX22" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="BY22" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="BZ22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA22" s="7">
+        <v>41505.0</v>
+      </c>
+      <c r="CB22" s="7">
+        <v>44105.0</v>
+      </c>
+      <c r="CC22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CD22" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="CE22" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="CF22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CG22" s="7">
+        <v>44105.0</v>
+      </c>
+      <c r="CI22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DL22" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="DM22" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN22" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="DO22" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="DP22" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="DT22" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="DU22" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1g6I2M1sVqCo3TwlnJ67zQPrjum4S8IYZ","Inscrição DOUTORADO PPGEM EEL-USP - Daniel Alexandre da Costa Ximenes.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Daniel Alexandre da Costa Ximenes.pdf</v>
+      </c>
+      <c r="DV22" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/183f1d68ee129960","Email sent to ppgem-eel@usp.br, danielacximenes@gmail.com")</f>
+        <v>Email sent to ppgem-eel@usp.br, danielacximenes@gmail.com</v>
+      </c>
+      <c r="DW22" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="DX22" s="9" t="s">
+        <v>598</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -7450,9 +8103,17 @@
     <hyperlink r:id="rId64" ref="DP20"/>
     <hyperlink r:id="rId65" ref="DT20"/>
     <hyperlink r:id="rId66" ref="DX20"/>
+    <hyperlink r:id="rId67" ref="DO21"/>
+    <hyperlink r:id="rId68" ref="DP21"/>
+    <hyperlink r:id="rId69" ref="DT21"/>
+    <hyperlink r:id="rId70" ref="DX21"/>
+    <hyperlink r:id="rId71" ref="DO22"/>
+    <hyperlink r:id="rId72" ref="DP22"/>
+    <hyperlink r:id="rId73" ref="DT22"/>
+    <hyperlink r:id="rId74" ref="DX22"/>
   </hyperlinks>
-  <drawing r:id="rId67"/>
-  <legacyDrawing r:id="rId68"/>
+  <drawing r:id="rId75"/>
+  <legacyDrawing r:id="rId76"/>
 </worksheet>
 </file>
 
@@ -7471,193 +8132,222 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>566</v>
+        <v>599</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>567</v>
+        <v>600</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>44830.76710104167</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>568</v>
+        <v>601</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>44784.87304421296</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>569</v>
+        <v>602</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>44784.87274673611</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>570</v>
+        <v>603</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>571</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>44770.501262986116</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>572</v>
+        <v>605</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>44757.68569034722</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>573</v>
+        <v>606</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>44756.72330104167</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>603</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>44649.34401880787</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>575</v>
+        <v>608</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44649.343747569445</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>576</v>
-      </c>
+        <v>609</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44648.7586062037</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>577</v>
+        <v>610</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44648.75839336806</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>578</v>
-      </c>
+        <v>611</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44376.74045414352</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>579</v>
+        <v>603</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44400.52960546296</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>578</v>
-      </c>
+        <v>613</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44400.5298077662</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>581</v>
+        <v>614</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44434.96399693287</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>582</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44434.96418570602</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>583</v>
+        <v>603</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>581</v>
+        <v>614</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44497.47637053241</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>584</v>
+        <v>616</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44509.64800585648</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>585</v>
+        <v>603</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44511.67887549769</v>
+        <v>44434.96418570602</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>570</v>
+        <v>619</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>578</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6">
+        <v>44497.47637053241</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6">
+        <v>44509.64800585648</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>586</v>
+      <c r="B23" s="2" t="s">
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2022-11-03 13:00:52 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -443,12 +443,37 @@
         <t xml:space="preserve">Updated on 19-Oct-2022 05:01 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT23">
+      <text>
+        <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU23">
+      <text>
+        <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV23">
+      <text>
+        <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW23">
+      <text>
+        <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX23">
+      <text>
+        <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="648">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2249,10 +2274,85 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnue9bYR30NiS5xhgj_0cGTLQCas0WK2AiqdNcGtwRoEkyFP5N_e_c110Pz35FCXg9qQ&amp;source=documentstudio&amp;timestamp=1666209668734</t>
   </si>
   <si>
+    <t>Marcel Demarco de Souza Oliveira</t>
+  </si>
+  <si>
+    <t>marcel.demarco@usp.br</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Volta Redonda - RJ</t>
+  </si>
+  <si>
+    <t>RJ/ Brasil</t>
+  </si>
+  <si>
+    <t>07896955709</t>
+  </si>
+  <si>
+    <t>IFP</t>
+  </si>
+  <si>
+    <t>Rua Juiz Nilton Leite, 141,ap.201</t>
+  </si>
+  <si>
+    <t>Jardim Primavera</t>
+  </si>
+  <si>
+    <t>Marcela Maria Santagueda</t>
+  </si>
+  <si>
+    <t>esposa</t>
+  </si>
+  <si>
+    <t>Rua Juiz Nilton Leite, 141, ap.201</t>
+  </si>
+  <si>
+    <t>USP - EEL</t>
+  </si>
+  <si>
+    <t>mestre em engenharia de materiais</t>
+  </si>
+  <si>
+    <t>ingles</t>
+  </si>
+  <si>
+    <t>CSN CIMENTOS BRASIL S.A</t>
+  </si>
+  <si>
+    <t>Supervisor da qualidade</t>
+  </si>
+  <si>
+    <t>melhores possiveis</t>
+  </si>
+  <si>
+    <t>ESTUDO DOS MECANISMOS DE HIDRATAÇÃO E NO DESEMPENHO DAS RESISTÊNCAS MECÂNICAS À COMPRESSÃO EM ARGAMASSAS DE CIMENTO SEM CLÍNQUER COM DIFERENTES COMPOSIÇÕES</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1NxlmlGj1eRaDi8uG8FiIHOpg1HFjnmex</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1KDGAqOLmePRtNo3hltEr-fn2lAItjx-W</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1b5GBMGqwBwq_C6LEEbz_IM4nIzlT4bU8</t>
+  </si>
+  <si>
+    <t>2_ABaOnudnoHdQthnGVO3Jq_evEi8NSQ0BdiQ29HUN5g6TQdcY_eLg2T-VhL_udOxT9UbZTyM</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnudnoHdQthnGVO3Jq_evEi8NSQ0BdiQ29HUN5g6TQdcY_eLg2T-VhL_udOxT9UbZTyM&amp;source=documentstudio&amp;timestamp=1667391485132</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #23 by luizeleno@usp.br</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #22 by luizeleno@usp.br</t>
@@ -8036,6 +8136,187 @@
         <v>598</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="6">
+        <v>44867.38755939815</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="I23" s="7">
+        <v>28957.0</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1.09600478E8</v>
+      </c>
+      <c r="N23" s="7">
+        <v>34684.0</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="P23" s="2">
+        <v>9121770.0</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="T23" s="2">
+        <v>2.728343E7</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V23" s="2">
+        <v>2.4999911461E10</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>2.728343E7</v>
+      </c>
+      <c r="AD23" s="2">
+        <v>2.49969492E9</v>
+      </c>
+      <c r="AE23" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="AG23" s="7">
+        <v>43682.0</v>
+      </c>
+      <c r="AH23" s="7">
+        <v>44523.0</v>
+      </c>
+      <c r="AI23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX23" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="AY23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR23" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="BS23" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="BT23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU23" s="7">
+        <v>38307.0</v>
+      </c>
+      <c r="BW23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DL23" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="DM23" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN23" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="DO23" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="DP23" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="DT23" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="DU23" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1b5GBMGqwBwq_C6LEEbz_IM4nIzlT4bU8","Inscrição DOUTORADO PPGEM EEL-USP - Marcel Demarco de Souza Oliveira.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Marcel Demarco de Souza Oliveira.pdf</v>
+      </c>
+      <c r="DV23" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/1843847bbab100c3","Email sent to ppgem-eel@usp.br, marcel.demarco@usp.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, marcel.demarco@usp.br</v>
+      </c>
+      <c r="DW23" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="DX23" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -8111,9 +8392,13 @@
     <hyperlink r:id="rId72" ref="DP22"/>
     <hyperlink r:id="rId73" ref="DT22"/>
     <hyperlink r:id="rId74" ref="DX22"/>
+    <hyperlink r:id="rId75" ref="DO23"/>
+    <hyperlink r:id="rId76" ref="DP23"/>
+    <hyperlink r:id="rId77" ref="DT23"/>
+    <hyperlink r:id="rId78" ref="DX23"/>
   </hyperlinks>
-  <drawing r:id="rId75"/>
-  <legacyDrawing r:id="rId76"/>
+  <drawing r:id="rId79"/>
+  <legacyDrawing r:id="rId80"/>
 </worksheet>
 </file>
 
@@ -8132,222 +8417,231 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>599</v>
+        <v>623</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>600</v>
+        <v>624</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>44853.70966662037</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>601</v>
+        <v>625</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>44853.694473275464</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>602</v>
+        <v>626</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>44853.69422237268</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>604</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>44830.76710104167</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>628</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>44784.87304421296</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>606</v>
+        <v>630</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>44784.87274673611</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>607</v>
-      </c>
+        <v>631</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>44770.501262986116</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>628</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44757.68569034722</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>609</v>
+        <v>633</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44756.72330104167</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>610</v>
+        <v>634</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44649.34401880787</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>611</v>
+        <v>635</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44649.343747569445</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>612</v>
-      </c>
+        <v>636</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44648.7586062037</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>628</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44648.75839336806</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>614</v>
-      </c>
+        <v>638</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44376.74045414352</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>615</v>
+        <v>628</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44400.52960546296</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>614</v>
+        <v>640</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44400.5298077662</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>616</v>
+        <v>628</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>617</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44434.96399693287</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>603</v>
+        <v>641</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>618</v>
+        <v>642</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44434.96418570602</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>617</v>
+        <v>643</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44497.47637053241</v>
+        <v>44434.96418570602</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>620</v>
+        <v>644</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44509.64800585648</v>
+        <v>44497.47637053241</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>621</v>
+        <v>645</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44511.67887549769</v>
+        <v>44509.64800585648</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>614</v>
+        <v>646</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>622</v>
+      <c r="B24" s="2" t="s">
+        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-05-26 13:00:12 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -468,12 +468,37 @@
         <t xml:space="preserve">Updated on 02-Nov-2022 09:18 AM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT24">
+      <text>
+        <t xml:space="preserve">Updated on 25-May-2023 03:49 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU24">
+      <text>
+        <t xml:space="preserve">Updated on 25-May-2023 03:49 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV24">
+      <text>
+        <t xml:space="preserve">Updated on 25-May-2023 03:49 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW24">
+      <text>
+        <t xml:space="preserve">Updated on 25-May-2023 03:48 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX24">
+      <text>
+        <t xml:space="preserve">Updated on 25-May-2023 03:48 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="673">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2346,12 +2371,91 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnudnoHdQthnGVO3Jq_evEi8NSQ0BdiQ29HUN5g6TQdcY_eLg2T-VhL_udOxT9UbZTyM&amp;source=documentstudio&amp;timestamp=1667391485132</t>
   </si>
   <si>
+    <t>Thaís Leite Garcia Nunes</t>
+  </si>
+  <si>
+    <t>thais.slgarcia@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>Rua José Maria Candreva, 86, 02</t>
+  </si>
+  <si>
+    <t>Jardim Amália</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Esposo</t>
+  </si>
+  <si>
+    <t>Universidade Federal Rural do Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Bacharel</t>
+  </si>
+  <si>
+    <t>Academia Militar das Agulhas Negras</t>
+  </si>
+  <si>
+    <t>Chefe de Estação de Tratamento de Água</t>
+  </si>
+  <si>
+    <t>Centro Universitário de Barra Mansa</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docente </t>
+  </si>
+  <si>
+    <t>Escola Técnica Pandiá Calógeras</t>
+  </si>
+  <si>
+    <t>Professora</t>
+  </si>
+  <si>
+    <t>Instituto de Cultura Técnica</t>
+  </si>
+  <si>
+    <t>Aprender e atuar com um excelente corpo docente e equipamentos em laboratórios de qualidade.</t>
+  </si>
+  <si>
+    <t>Ainda não tenho projeto. Estou tentando contato com professor.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1dowNVC-gRnkdkZWiOj75oOm8DOj_D3gS</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1sezkqEUNZajA1o8dJ4jyqyTchzypx1xY</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1YHqMTQ0oldHahxYrxAly9-6KOsi8pVm1</t>
+  </si>
+  <si>
+    <t>2_ABaOnuf_rCqzF6ZeYFSWehwNQTBhvBn9V1p239bNg_tqFExXQYhyJ6Q-_ueurR-aVcNosGI</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnuf_rCqzF6ZeYFSWehwNQTBhvBn9V1p239bNg_tqFExXQYhyJ6Q-_ueurR-aVcNosGI&amp;source=documentstudio&amp;timestamp=1685040490412</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
   </si>
   <si>
+    <t>✔️  [Respostas] Processed form row #24 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>⚠️  Google Form has duplicate question titles</t>
+  </si>
+  <si>
+    <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')
+inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
+  </si>
+  <si>
     <t>✔️  [Respostas] Processed form row #23 by luizeleno@usp.br</t>
   </si>
   <si>
@@ -2359,9 +2463,6 @@
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #21 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>⚠️  Google Form has duplicate question titles</t>
   </si>
   <si>
     <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')</t>
@@ -8317,6 +8418,286 @@
         <v>622</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="6">
+        <v>45071.658453842596</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I24" s="7">
+        <v>30950.0</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.0882591703E10</v>
+      </c>
+      <c r="M24" s="2">
+        <v>2.01588811E8</v>
+      </c>
+      <c r="N24" s="7">
+        <v>43584.0</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T24" s="2">
+        <v>2.7251188E7</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V24" s="2">
+        <v>2.4992519411E10</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>2.7251188E7</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>2.4999628219E10</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG24" s="7">
+        <v>40575.0</v>
+      </c>
+      <c r="AH24" s="7">
+        <v>41414.0</v>
+      </c>
+      <c r="AI24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="AK24" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="AL24" s="7">
+        <v>38078.0</v>
+      </c>
+      <c r="AM24" s="7">
+        <v>40532.0</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BB24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR24" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="BS24" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="BT24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU24" s="7">
+        <v>44682.0</v>
+      </c>
+      <c r="BW24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX24" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="BY24" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="BZ24" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA24" s="7">
+        <v>41426.0</v>
+      </c>
+      <c r="CB24" s="7">
+        <v>44216.0</v>
+      </c>
+      <c r="CC24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP24" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="CQ24" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="CR24" s="7">
+        <v>41426.0</v>
+      </c>
+      <c r="CS24" s="7">
+        <v>44216.0</v>
+      </c>
+      <c r="CT24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU24" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="CV24" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="CW24" s="7">
+        <v>41671.0</v>
+      </c>
+      <c r="CX24" s="7">
+        <v>42399.0</v>
+      </c>
+      <c r="CY24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CZ24" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="DA24" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="DB24" s="7">
+        <v>40940.0</v>
+      </c>
+      <c r="DC24" s="7">
+        <v>41993.0</v>
+      </c>
+      <c r="DD24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL24" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="DM24" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="DN24" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="DO24" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="DP24" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="DQ24" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR24" s="2">
+        <v>15830.0</v>
+      </c>
+      <c r="DS24" s="2">
+        <v>711101.0</v>
+      </c>
+      <c r="DT24" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="DU24" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1YHqMTQ0oldHahxYrxAly9-6KOsi8pVm1","Inscrição DOUTORADO PPGEM EEL-USP - Thaís Leite Garcia Nunes.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Thaís Leite Garcia Nunes.pdf</v>
+      </c>
+      <c r="DV24" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/188543e46f563d12","Email sent to ppgem-eel@usp.br, thais.slgarcia@yahoo.com.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, thais.slgarcia@yahoo.com.br</v>
+      </c>
+      <c r="DW24" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="DX24" s="9" t="s">
+        <v>645</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -8396,9 +8777,13 @@
     <hyperlink r:id="rId76" ref="DP23"/>
     <hyperlink r:id="rId77" ref="DT23"/>
     <hyperlink r:id="rId78" ref="DX23"/>
+    <hyperlink r:id="rId79" ref="DO24"/>
+    <hyperlink r:id="rId80" ref="DP24"/>
+    <hyperlink r:id="rId81" ref="DT24"/>
+    <hyperlink r:id="rId82" ref="DX24"/>
   </hyperlinks>
-  <drawing r:id="rId79"/>
-  <legacyDrawing r:id="rId80"/>
+  <drawing r:id="rId83"/>
+  <legacyDrawing r:id="rId84"/>
 </worksheet>
 </file>
 
@@ -8417,231 +8802,251 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>623</v>
+        <v>646</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>624</v>
+        <v>647</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>44867.38816256945</v>
+        <v>45071.65914045139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>625</v>
+        <v>648</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>44853.70966662037</v>
+        <v>45071.658906192126</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>649</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>44853.694473275464</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>627</v>
+        <v>651</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>44853.69422237268</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>629</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>44830.76710104167</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>44784.87304421296</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>649</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>44784.87274673611</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>632</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44770.501262986116</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>633</v>
+        <v>656</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44757.68569034722</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>649</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44756.72330104167</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>635</v>
+        <v>658</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44649.34401880787</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>636</v>
+        <v>659</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44649.343747569445</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>637</v>
-      </c>
+        <v>660</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44648.7586062037</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>638</v>
+        <v>661</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44648.75839336806</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>628</v>
+        <v>649</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>639</v>
+        <v>662</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44376.74045414352</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>640</v>
-      </c>
+        <v>663</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44400.52960546296</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>628</v>
+        <v>649</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>639</v>
+        <v>664</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44400.5298077662</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>642</v>
+        <v>665</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44434.96399693287</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>628</v>
+        <v>649</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>643</v>
+        <v>664</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44434.96418570602</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>644</v>
+        <v>666</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>642</v>
+        <v>667</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44497.47637053241</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>645</v>
+        <v>649</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44509.64800585648</v>
+        <v>44434.96418570602</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>646</v>
+        <v>669</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6">
-        <v>44511.67887549769</v>
+        <v>44497.47637053241</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>639</v>
+        <v>670</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6">
+        <v>44509.64800585648</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>647</v>
+      <c r="B26" s="2" t="s">
+        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-06-01 19:00:13 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -493,12 +493,37 @@
         <t xml:space="preserve">Updated on 25-May-2023 03:48 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT25">
+      <text>
+        <t xml:space="preserve">Updated on 01-Jun-2023 02:44 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU25">
+      <text>
+        <t xml:space="preserve">Updated on 01-Jun-2023 02:44 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV25">
+      <text>
+        <t xml:space="preserve">Updated on 01-Jun-2023 02:44 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW25">
+      <text>
+        <t xml:space="preserve">Updated on 01-Jun-2023 02:43 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX25">
+      <text>
+        <t xml:space="preserve">Updated on 01-Jun-2023 02:43 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="697">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2440,10 +2465,82 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnuf_rCqzF6ZeYFSWehwNQTBhvBn9V1p239bNg_tqFExXQYhyJ6Q-_ueurR-aVcNosGI&amp;source=documentstudio&amp;timestamp=1685040490412</t>
   </si>
   <si>
+    <t>Jéssica Vicente Luiz</t>
+  </si>
+  <si>
+    <t>jessica.vluiz@usp.br</t>
+  </si>
+  <si>
+    <t>Detran/RJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenida Oswaldo Aranha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bairro da Cruz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorena </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcello Salerno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namorado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Oswaldo Aranha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP/Brasil </t>
+  </si>
+  <si>
+    <t>Escola de Engenharia de Lorena - USP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mestre em Engenharia de Materiais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eletronuclear - Eletrobrás </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estagiário </t>
+  </si>
+  <si>
+    <t>Desenvolver as minhas habilidades profissionais na área de pesquisa e ensino.</t>
+  </si>
+  <si>
+    <t>Avaliação experimental e modelagem termodinâmica do sistema Al-Hf-Ti</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1SYAePs3M-y8V4y3SE5yUQpfT-RXpVKDM</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1UD-D4FSD0ucMEvz3bTGSRmFNqXnLW7fA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco do Brasil </t>
+  </si>
+  <si>
+    <t>0460-X</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1cEP188shzsBUx3nuOHYcW-TckVM-dmmI</t>
+  </si>
+  <si>
+    <t>2_ABaOnucuwKh4sG_Boyz65yJ9CzmABswx259nDNr5ZZeNcG44ctPASfA62vczs_omASUQym0</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnucuwKh4sG_Boyz65yJ9CzmABswx259nDNr5ZZeNcG44ctPASfA62vczs_omASUQym0&amp;source=documentstudio&amp;timestamp=1685641413499</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #25 by luizeleno@usp.br</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #24 by luizeleno@usp.br</t>
@@ -8698,6 +8795,199 @@
         <v>645</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="6">
+        <v>45078.613582164355</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="7">
+        <v>34750.0</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.5105963725E10</v>
+      </c>
+      <c r="M25" s="2">
+        <v>2.32763888E8</v>
+      </c>
+      <c r="N25" s="7">
+        <v>41401.0</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1.2424371E7</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="T25" s="2">
+        <v>1.2606E7</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V25" s="2">
+        <v>2.4998194964E10</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>1.2606E7</v>
+      </c>
+      <c r="AD25" s="2">
+        <v>1.2996680886E10</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="AG25" s="7">
+        <v>44257.0</v>
+      </c>
+      <c r="AH25" s="7">
+        <v>45072.0</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR25" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="BS25" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="BT25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BU25" s="7">
+        <v>43626.0</v>
+      </c>
+      <c r="BV25" s="7">
+        <v>44253.0</v>
+      </c>
+      <c r="BW25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL25" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="DM25" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN25" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="DO25" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="DP25" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="DQ25" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="DR25" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="DS25" s="2">
+        <v>619752.0</v>
+      </c>
+      <c r="DT25" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="DU25" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1cEP188shzsBUx3nuOHYcW-TckVM-dmmI","Inscrição DOUTORADO PPGEM EEL-USP - Jéssica Vicente Luiz.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Jéssica Vicente Luiz.pdf</v>
+      </c>
+      <c r="DV25" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/188780f5e4c26a1a","Email sent to ppgem-eel@usp.br, jessica.vluiz@usp.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, jessica.vluiz@usp.br</v>
+      </c>
+      <c r="DW25" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="DX25" s="9" t="s">
+        <v>668</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -8781,9 +9071,13 @@
     <hyperlink r:id="rId80" ref="DP24"/>
     <hyperlink r:id="rId81" ref="DT24"/>
     <hyperlink r:id="rId82" ref="DX24"/>
+    <hyperlink r:id="rId83" ref="DO25"/>
+    <hyperlink r:id="rId84" ref="DP25"/>
+    <hyperlink r:id="rId85" ref="DT25"/>
+    <hyperlink r:id="rId86" ref="DX25"/>
   </hyperlinks>
-  <drawing r:id="rId83"/>
-  <legacyDrawing r:id="rId84"/>
+  <drawing r:id="rId87"/>
+  <legacyDrawing r:id="rId88"/>
 </worksheet>
 </file>
 
@@ -8802,251 +9096,260 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>646</v>
+        <v>669</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>647</v>
+        <v>670</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>45071.65914045139</v>
+        <v>45078.61406284722</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>648</v>
+        <v>671</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>45071.658906192126</v>
+        <v>45071.65914045139</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>650</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>44867.38816256945</v>
+        <v>45071.658906192126</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>673</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>44853.70966662037</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>652</v>
+        <v>675</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>44853.694473275464</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>653</v>
+        <v>676</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>44853.69422237268</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>654</v>
-      </c>
+        <v>677</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>44830.76710104167</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>673</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44784.87304421296</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>656</v>
+        <v>679</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44784.87274673611</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>657</v>
-      </c>
+        <v>680</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44770.501262986116</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>673</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44757.68569034722</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>659</v>
+        <v>682</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44756.72330104167</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>660</v>
+        <v>683</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44649.34401880787</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>661</v>
+        <v>684</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44649.343747569445</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>662</v>
-      </c>
+        <v>685</v>
+      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44648.7586062037</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>673</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44648.75839336806</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>664</v>
-      </c>
+        <v>687</v>
+      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44376.74045414352</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>665</v>
+        <v>673</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44400.52960546296</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>664</v>
+        <v>689</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44400.5298077662</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>667</v>
+        <v>688</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44434.96399693287</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>649</v>
+        <v>690</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>668</v>
+        <v>691</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44434.96418570602</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>667</v>
+        <v>692</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6">
-        <v>44497.47637053241</v>
+        <v>44434.96418570602</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>670</v>
+        <v>693</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6">
-        <v>44509.64800585648</v>
+        <v>44497.47637053241</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6">
-        <v>44511.67887549769</v>
+        <v>44509.64800585648</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>664</v>
+        <v>695</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>672</v>
+      <c r="B27" s="2" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-10-31 13:00:27 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -518,12 +518,62 @@
         <t xml:space="preserve">Updated on 01-Jun-2023 02:43 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT26">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 10:26 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU26">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 10:26 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV26">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 10:26 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW26">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 10:26 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX26">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 10:26 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DT27">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU27">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV27">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW27">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX27">
+      <text>
+        <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="747">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2534,19 +2584,172 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnucuwKh4sG_Boyz65yJ9CzmABswx259nDNr5ZZeNcG44ctPASfA62vczs_omASUQym0&amp;source=documentstudio&amp;timestamp=1685641413499</t>
   </si>
   <si>
+    <t>Diego Magalhães Baía</t>
+  </si>
+  <si>
+    <t>diegobaia@id.uff.br</t>
+  </si>
+  <si>
+    <t>DETRAN-RJ</t>
+  </si>
+  <si>
+    <t>Av. Waldomiro Peres Gonçalves, 3200. Casa 02</t>
+  </si>
+  <si>
+    <t>Mangueira</t>
+  </si>
+  <si>
+    <t>Avenida Waldomiro Peres Gonçalves, 3200. Casa 02</t>
+  </si>
+  <si>
+    <t>Universidade Federal Fluminense (UFF)</t>
+  </si>
+  <si>
+    <t>Grupo OPUS</t>
+  </si>
+  <si>
+    <t>Analista de Produtos</t>
+  </si>
+  <si>
+    <t>Bolsista</t>
+  </si>
+  <si>
+    <t>Estágio em Docência</t>
+  </si>
+  <si>
+    <t>Obtenção do título de doutor com bom desenvolvimento profissional e acadêmico, aprimorando minhas habilidades técnicas, acadêmicas e de ensino em uma instituição de qualidade e grande relevância.</t>
+  </si>
+  <si>
+    <t>Escola onde estudo</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de ligas à base de Mg-Al-Mn com adição de Ca</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1h-lAzOkmUqEy4FvO-3SghVkM3HTYh1Xu</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=199XQxxTW9hpeWnBvw95mL6GrjBwMG3A1</t>
+  </si>
+  <si>
+    <t>2922-X</t>
+  </si>
+  <si>
+    <t>46.198-9</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1edQHOGyoIKhxiR-AF-rt5QiTmd3QDR-F</t>
+  </si>
+  <si>
+    <t>2_ABaOnufMJ2tCDJiQkepRBd6avG5YRQucNPaBlzOGJ1eFffZEltWzapF5kZEYOuoKbBeIuok</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnufMJ2tCDJiQkepRBd6avG5YRQucNPaBlzOGJ1eFffZEltWzapF5kZEYOuoKbBeIuok&amp;source=documentstudio&amp;timestamp=1698672359458</t>
+  </si>
+  <si>
+    <t>Everton Diniz dos Santos</t>
+  </si>
+  <si>
+    <t>ediniz@id.uff.br</t>
+  </si>
+  <si>
+    <t>Rua Nelson Godoy,260</t>
+  </si>
+  <si>
+    <t>Paraíso</t>
+  </si>
+  <si>
+    <t>Resende-RJ</t>
+  </si>
+  <si>
+    <t>Luiz Carlos</t>
+  </si>
+  <si>
+    <t>Rua Nelson Godoy,266</t>
+  </si>
+  <si>
+    <t>UNESA</t>
+  </si>
+  <si>
+    <t>Bacharel/Farmácia</t>
+  </si>
+  <si>
+    <t>UNIVAP</t>
+  </si>
+  <si>
+    <t>Doutorado/Engenharia biomédica</t>
+  </si>
+  <si>
+    <t>Mestre/Ciências biológicas</t>
+  </si>
+  <si>
+    <t>Bacharel/Biomedicina</t>
+  </si>
+  <si>
+    <t>Docente de matemática/química no E.M.</t>
+  </si>
+  <si>
+    <t>UNIFOA</t>
+  </si>
+  <si>
+    <t>Docente no ensino superior</t>
+  </si>
+  <si>
+    <t>NANOCORDAS (Minha startup)</t>
+  </si>
+  <si>
+    <t>Diretor</t>
+  </si>
+  <si>
+    <t>Docente e coordenador (Biomedicina)</t>
+  </si>
+  <si>
+    <t>Docente e coordenador de curso</t>
+  </si>
+  <si>
+    <t>Estou a frente de uma startup que produz materiais antimicrobianos por meio de processos a plasma. A alguns anos perdi um ente querido por agravo de infecção nosocomial. Desde então tenho como missão de vida usar a nanotecnologia para resolver este problema. Assim desenvolvi, com recursos pessoais e na pequena cidade de Resende-RJ, um sistema hibrido PVD/PECVD. No meu reator eu desenvolvi roupas e talheres antimicrobianos, para uso em ambiente hospitalar. Estou nesta jornada sozinho desde 2019 e enfrento muitos desafios, tanto financeiros quanto técnicos posto que não há com quem eu possa discutir, sem conflito de interesses, sobre os desafios e resultados logrados. Desse modo, minhas expectativas ao me candidatar para este doutorado são muitas, dentre as quais destaco as seguintes: - Ter acesso a laboratórios e equipamentos para caracterização de materiais; - Elevar significativamente meu número de publicações e citações recebidas; - receber orientações de um mentor com grande conhecimento em eng. de materiais; - me integrar a um bom grupo de pesquisa, preferencialmente com interdisciplinaridade entre seus integrantes, para ter novas ideias de pesquisas/potenciais soluções para problemas de materiais de uso hospitalar. Creio que todas as expectativas confluem para o meu objetivo enquanto estudante, que é o de transferir conhecimentos gerados nos bancos da universidade, para o benefício da sociedade. E isto somente é feito por meio do empreendedorismo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talheres anti-patogênicos por ação de filme nanoestruturado de "diamond-like carbon" </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1RtCazJHxhoY3IL3XwIarJxVVoGEigTht</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1phDyuQTU5TU-TZQZq3d2RCoyk51C-z18</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1KyR-cSrnzqX7-Dh2PhDriR2NFVgMWDl7</t>
+  </si>
+  <si>
+    <t>2_ABaOnufMMVG5f-zAervGJfgz3lDDjuArQO5Bqj0AksNE4YYYspPgjTX2uG5vnBqN2o68OtU</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnufMMVG5f-zAervGJfgz3lDDjuArQO5Bqj0AksNE4YYYspPgjTX2uG5vnBqN2o68OtU&amp;source=documentstudio&amp;timestamp=1698700202835</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
   </si>
   <si>
+    <t>✔️  [Respostas] Processed form row #27 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>⚠️  Google Form has duplicate question titles</t>
+  </si>
+  <si>
+    <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #26 by luizeleno@usp.br</t>
+  </si>
+  <si>
     <t>✔️  [Respostas] Processed form row #25 by luizeleno@usp.br</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #24 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>⚠️  Google Form has duplicate question titles</t>
   </si>
   <si>
     <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')
@@ -2560,9 +2763,6 @@
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #21 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #20 by luizeleno@usp.br</t>
@@ -8988,6 +9188,563 @@
         <v>668</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="6">
+        <v>45229.43471594907</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I26" s="7">
+        <v>34429.0</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1.2382276789E10</v>
+      </c>
+      <c r="M26" s="2">
+        <v>2.3089814E8</v>
+      </c>
+      <c r="N26" s="7">
+        <v>41404.0</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="T26" s="2">
+        <v>2.7333002E7</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V26" s="2">
+        <v>2.499997352E10</v>
+      </c>
+      <c r="W26" s="2">
+        <v>2.4999933482E10</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>2.7333002E7</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>2.4999933482E10</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG26" s="7">
+        <v>43717.0</v>
+      </c>
+      <c r="AH26" s="7">
+        <v>44770.0</v>
+      </c>
+      <c r="AI26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK26" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AL26" s="7">
+        <v>40973.0</v>
+      </c>
+      <c r="AM26" s="7">
+        <v>43454.0</v>
+      </c>
+      <c r="AN26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR26" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="BS26" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="BT26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU26" s="7">
+        <v>44936.0</v>
+      </c>
+      <c r="BW26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX26" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BY26" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="BZ26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="CA26" s="7">
+        <v>43922.0</v>
+      </c>
+      <c r="CB26" s="7">
+        <v>44620.0</v>
+      </c>
+      <c r="CC26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP26" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="CQ26" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="CR26" s="7">
+        <v>44490.0</v>
+      </c>
+      <c r="CS26" s="7">
+        <v>44604.0</v>
+      </c>
+      <c r="CT26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL26" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="DM26" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="DN26" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="DO26" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="DP26" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="DQ26" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR26" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="DS26" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="DT26" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="DU26" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1edQHOGyoIKhxiR-AF-rt5QiTmd3QDR-F","Inscrição DOUTORADO PPGEM EEL-USP - Diego Magalhães Baía.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Diego Magalhães Baía.pdf</v>
+      </c>
+      <c r="DV26" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18b80c3e04cd69ef","Email sent to ppgem-eel@usp.br, diegobaia@id.uff.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, diegobaia@id.uff.br</v>
+      </c>
+      <c r="DW26" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="DX26" s="9" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6">
+        <v>45229.75697725694</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="I27" s="7">
+        <v>31829.0</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1.1551904756E10</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1.3182233E8</v>
+      </c>
+      <c r="N27" s="7">
+        <v>36248.0</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="T27" s="2">
+        <v>2.753604E7</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V27" s="2">
+        <v>1.2981929195E10</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>2.753604E7</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>2.4981189841E10</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="AG27" s="7">
+        <v>44593.0</v>
+      </c>
+      <c r="AH27" s="7">
+        <v>44958.0</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="AL27" s="7">
+        <v>41306.0</v>
+      </c>
+      <c r="AM27" s="7">
+        <v>42583.0</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO27" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="AQ27" s="7">
+        <v>42767.0</v>
+      </c>
+      <c r="AR27" s="7">
+        <v>43435.0</v>
+      </c>
+      <c r="AS27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT27" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AU27" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="AV27" s="7">
+        <v>39114.0</v>
+      </c>
+      <c r="AW27" s="7">
+        <v>40513.0</v>
+      </c>
+      <c r="AX27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD27" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE27" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BF27" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BG27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR27" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS27" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="BT27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU27" s="7">
+        <v>42887.0</v>
+      </c>
+      <c r="BV27" s="7">
+        <v>43160.0</v>
+      </c>
+      <c r="BW27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX27" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="BY27" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="BZ27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA27" s="7">
+        <v>43132.0</v>
+      </c>
+      <c r="CB27" s="7">
+        <v>43497.0</v>
+      </c>
+      <c r="CC27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CD27" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="CE27" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="CF27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CG27" s="7">
+        <v>43617.0</v>
+      </c>
+      <c r="CI27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CJ27" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="CK27" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="CL27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CM27" s="7">
+        <v>43497.0</v>
+      </c>
+      <c r="CN27" s="7">
+        <v>45228.0</v>
+      </c>
+      <c r="CO27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP27" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="CQ27" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="CR27" s="7">
+        <v>43497.0</v>
+      </c>
+      <c r="CT27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL27" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="DM27" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="DN27" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="DO27" s="9" t="s">
+        <v>712</v>
+      </c>
+      <c r="DP27" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="DQ27" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR27" s="2">
+        <v>33030.0</v>
+      </c>
+      <c r="DS27" s="2">
+        <v>155756.0</v>
+      </c>
+      <c r="DT27" s="9" t="s">
+        <v>714</v>
+      </c>
+      <c r="DU27" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1KyR-cSrnzqX7-Dh2PhDriR2NFVgMWDl7","Inscrição DOUTORADO PPGEM EEL-USP - Everton Diniz dos Santos.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Everton Diniz dos Santos.pdf</v>
+      </c>
+      <c r="DV27" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18b826ca45a375c6","Email sent to ppgem-eel@usp.br, ediniz@id.uff.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, ediniz@id.uff.br</v>
+      </c>
+      <c r="DW27" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="DX27" s="9" t="s">
+        <v>716</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -9075,9 +9832,17 @@
     <hyperlink r:id="rId84" ref="DP25"/>
     <hyperlink r:id="rId85" ref="DT25"/>
     <hyperlink r:id="rId86" ref="DX25"/>
+    <hyperlink r:id="rId87" ref="DO26"/>
+    <hyperlink r:id="rId88" ref="DP26"/>
+    <hyperlink r:id="rId89" ref="DT26"/>
+    <hyperlink r:id="rId90" ref="DX26"/>
+    <hyperlink r:id="rId91" ref="DO27"/>
+    <hyperlink r:id="rId92" ref="DP27"/>
+    <hyperlink r:id="rId93" ref="DT27"/>
+    <hyperlink r:id="rId94" ref="DX27"/>
   </hyperlinks>
-  <drawing r:id="rId87"/>
-  <legacyDrawing r:id="rId88"/>
+  <drawing r:id="rId95"/>
+  <legacyDrawing r:id="rId96"/>
 </worksheet>
 </file>
 
@@ -9096,260 +9861,300 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>669</v>
+        <v>717</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>670</v>
+        <v>718</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>45078.61406284722</v>
+        <v>45229.75742496528</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>671</v>
+        <v>719</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>45071.65914045139</v>
+        <v>45229.75720832176</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>720</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>45071.658906192126</v>
+        <v>45229.43523862268</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>674</v>
-      </c>
+        <v>722</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>44867.38816256945</v>
+        <v>45229.434958645834</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>720</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>44853.70966662037</v>
+        <v>45078.61406284722</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>676</v>
+        <v>723</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>44853.694473275464</v>
+        <v>45071.65914045139</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>677</v>
+        <v>724</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>44853.69422237268</v>
+        <v>45071.658906192126</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>673</v>
+        <v>720</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>678</v>
+        <v>725</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44830.76710104167</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>679</v>
+        <v>726</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44784.87304421296</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>680</v>
+        <v>727</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44784.87274673611</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>681</v>
-      </c>
+        <v>728</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44770.501262986116</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>682</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>720</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44757.68569034722</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>683</v>
+        <v>729</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44756.72330104167</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>684</v>
+        <v>730</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44649.34401880787</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>720</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44649.343747569445</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>686</v>
-      </c>
+        <v>732</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44648.7586062037</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>687</v>
+        <v>733</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44648.75839336806</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>688</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44376.74045414352</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>689</v>
-      </c>
+        <v>735</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44400.52960546296</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>673</v>
+        <v>720</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>688</v>
+        <v>736</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44400.5298077662</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>691</v>
-      </c>
+        <v>737</v>
+      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44434.96399693287</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>673</v>
+        <v>720</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>692</v>
+        <v>738</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6">
-        <v>44434.96418570602</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>693</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>691</v>
+        <v>739</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6">
-        <v>44497.47637053241</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>694</v>
+        <v>720</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6">
-        <v>44509.64800585648</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>695</v>
+        <v>740</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6">
-        <v>44511.67887549769</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>673</v>
+        <v>720</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>688</v>
+        <v>742</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6">
+        <v>44434.96418570602</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6">
+        <v>44497.47637053241</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6">
+        <v>44509.64800585648</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>696</v>
+      <c r="B31" s="2" t="s">
+        <v>746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-11-01 22:00:26 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -568,12 +568,37 @@
         <t xml:space="preserve">Updated on 30-Oct-2023 06:10 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT28">
+      <text>
+        <t xml:space="preserve">Updated on 31-Oct-2023 07:12 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU28">
+      <text>
+        <t xml:space="preserve">Updated on 31-Oct-2023 07:12 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV28">
+      <text>
+        <t xml:space="preserve">Updated on 31-Oct-2023 07:12 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW28">
+      <text>
+        <t xml:space="preserve">Updated on 31-Oct-2023 07:11 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX28">
+      <text>
+        <t xml:space="preserve">Updated on 31-Oct-2023 07:11 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="771">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2728,16 +2753,91 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnufMMVG5f-zAervGJfgz3lDDjuArQO5Bqj0AksNE4YYYspPgjTX2uG5vnBqN2o68OtU&amp;source=documentstudio&amp;timestamp=1698700202835</t>
   </si>
   <si>
+    <t>Bruno Abreu Bon</t>
+  </si>
+  <si>
+    <t>brunoab89@hotmail.com</t>
+  </si>
+  <si>
+    <t>Detran-RJ</t>
+  </si>
+  <si>
+    <t>Rua Tupi, 279</t>
+  </si>
+  <si>
+    <t>Vila Hepacare</t>
+  </si>
+  <si>
+    <t>Orestes Francisco Trindade</t>
+  </si>
+  <si>
+    <t>Amigo</t>
+  </si>
+  <si>
+    <t>Avenida Nossa Senhora do Amparo, 6253</t>
+  </si>
+  <si>
+    <t>Santa Rita do Zarur</t>
+  </si>
+  <si>
+    <t>Universidade de São Paulo</t>
+  </si>
+  <si>
+    <t>Mestrado em Ciência e Engenharia de Materiais</t>
+  </si>
+  <si>
+    <t>Bacharelado em Engenharia de Materiais</t>
+  </si>
+  <si>
+    <t>Fundação Cecierj</t>
+  </si>
+  <si>
+    <t>Tutor Presencial de Ciência dos Materiais</t>
+  </si>
+  <si>
+    <t>Monitor de Física I Experimental</t>
+  </si>
+  <si>
+    <t>Ampliação de conhecimento na Engenharia de Materiais, ter maior vivência em laboratório, apresentações e publicações em Congressos e Anais, tornando-se um profissional cada vez mais preparado como pesquisador e academicista.</t>
+  </si>
+  <si>
+    <t>ABORDAGEM MULTI-ESCALA PARA O DESENVOLVIMENTO DE REVESTIMENTOS PROTETIVOS DE ALUMINETOS VIA PACK CEMENTATION EM LIGAS γ-TiAl</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1c4T8TopIBnqT7jUqjTgXPXNUKRX8KJj_</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1N5zWCcIi0zfTCoXNiSewLSlazrcu5K77</t>
+  </si>
+  <si>
+    <t>2922X</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1hNtKLUBrfjc9_DU1ieibvgcOUkOONmu1</t>
+  </si>
+  <si>
+    <t>2_ABaOnuc7t411_eL6ysWa4cKfkru8dFWzjVg7XzuBbzvsn30d17uCDcpCv3T7eFcxDiBAj-0</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnuc7t411_eL6ysWa4cKfkru8dFWzjVg7XzuBbzvsn30d17uCDcpCv3T7eFcxDiBAj-0&amp;source=documentstudio&amp;timestamp=1698790269958</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
   </si>
   <si>
+    <t>✔️  [Respostas] Processed form row #28 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>⚠️  Google Form has duplicate question titles</t>
+  </si>
+  <si>
+    <t>inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
+  </si>
+  <si>
     <t>✔️  [Respostas] Processed form row #27 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>⚠️  Google Form has duplicate question titles</t>
   </si>
   <si>
     <t>adicionaroutroidioma (Value changed from 'Sim' to 'Não')</t>
@@ -2769,9 +2869,6 @@
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #19 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #18 in 64 seconds.</t>
@@ -9745,6 +9842,226 @@
         <v>716</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="6">
+        <v>45230.79942081019</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I28" s="7">
+        <v>32557.0</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1.1241262799E10</v>
+      </c>
+      <c r="M28" s="2">
+        <v>2.12455901E8</v>
+      </c>
+      <c r="N28" s="7">
+        <v>39205.0</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1.118961E7</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T28" s="2">
+        <v>1.2608345E7</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V28" s="2">
+        <v>2.4981113359E10</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="AA28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB28" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>2.7288001E7</v>
+      </c>
+      <c r="AD28" s="2">
+        <v>2.433372848E9</v>
+      </c>
+      <c r="AE28" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="AF28" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="AG28" s="7">
+        <v>43535.0</v>
+      </c>
+      <c r="AH28" s="7">
+        <v>45197.0</v>
+      </c>
+      <c r="AI28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ28" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="AK28" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="AL28" s="7">
+        <v>41281.0</v>
+      </c>
+      <c r="AM28" s="7">
+        <v>43449.0</v>
+      </c>
+      <c r="AN28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AZ28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP28" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="CQ28" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="CR28" s="7">
+        <v>44655.0</v>
+      </c>
+      <c r="CS28" s="7">
+        <v>44958.0</v>
+      </c>
+      <c r="CT28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU28" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="CV28" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="CW28" s="7">
+        <v>41774.0</v>
+      </c>
+      <c r="CX28" s="7">
+        <v>42357.0</v>
+      </c>
+      <c r="CY28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL28" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="DM28" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN28" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="DO28" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="DP28" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="DQ28" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR28" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="DS28" s="2">
+        <v>1087193.0</v>
+      </c>
+      <c r="DT28" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="DU28" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1hNtKLUBrfjc9_DU1ieibvgcOUkOONmu1","Inscrição DOUTORADO PPGEM EEL-USP - Bruno Abreu Bon.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Bruno Abreu Bon.pdf</v>
+      </c>
+      <c r="DV28" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18b87cb463a790bd","Email sent to ppgem-eel@usp.br, brunoab89@hotmail.com")</f>
+        <v>Email sent to ppgem-eel@usp.br, brunoab89@hotmail.com</v>
+      </c>
+      <c r="DW28" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="DX28" s="9" t="s">
+        <v>739</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -9840,9 +10157,13 @@
     <hyperlink r:id="rId92" ref="DP27"/>
     <hyperlink r:id="rId93" ref="DT27"/>
     <hyperlink r:id="rId94" ref="DX27"/>
+    <hyperlink r:id="rId95" ref="DO28"/>
+    <hyperlink r:id="rId96" ref="DP28"/>
+    <hyperlink r:id="rId97" ref="DT28"/>
+    <hyperlink r:id="rId98" ref="DX28"/>
   </hyperlinks>
-  <drawing r:id="rId95"/>
-  <legacyDrawing r:id="rId96"/>
+  <drawing r:id="rId99"/>
+  <legacyDrawing r:id="rId100"/>
 </worksheet>
 </file>
 
@@ -9861,300 +10182,320 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>717</v>
+        <v>740</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>718</v>
+        <v>741</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>45229.75742496528</v>
+        <v>45230.80012315972</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>719</v>
+        <v>742</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>45229.75720832176</v>
+        <v>45230.79985361111</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>721</v>
+        <v>744</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>45229.43523862268</v>
+        <v>45229.75742496528</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>722</v>
+        <v>745</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>45229.434958645834</v>
+        <v>45229.75720832176</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>721</v>
+        <v>746</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>45078.61406284722</v>
+        <v>45229.43523862268</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>723</v>
+        <v>747</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>45071.65914045139</v>
+        <v>45229.434958645834</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>724</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>743</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>45071.658906192126</v>
+        <v>45078.61406284722</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>725</v>
-      </c>
+        <v>748</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>44867.38816256945</v>
+        <v>45071.65914045139</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>726</v>
+        <v>749</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>44853.70966662037</v>
+        <v>45071.658906192126</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>743</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44853.694473275464</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>728</v>
+        <v>751</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44853.69422237268</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>721</v>
-      </c>
+        <v>752</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44830.76710104167</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>729</v>
+        <v>753</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44784.87304421296</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>730</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>743</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44784.87274673611</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>731</v>
-      </c>
+        <v>754</v>
+      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44770.501262986116</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>732</v>
+        <v>755</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44757.68569034722</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>733</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>743</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44756.72330104167</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>734</v>
+        <v>756</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44649.34401880787</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>735</v>
+        <v>757</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44649.343747569445</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>736</v>
-      </c>
+        <v>758</v>
+      </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44648.7586062037</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>737</v>
+        <v>759</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44648.75839336806</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>738</v>
+        <v>760</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6">
-        <v>44376.74045414352</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>739</v>
-      </c>
+        <v>761</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="6">
-        <v>44400.52960546296</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>738</v>
+        <v>762</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6">
-        <v>44400.5298077662</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>741</v>
+        <v>763</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6">
-        <v>44434.96399693287</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>720</v>
+        <v>743</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>742</v>
+        <v>762</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6">
-        <v>44434.96418570602</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>743</v>
+        <v>764</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>741</v>
+        <v>765</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6">
-        <v>44497.47637053241</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6">
-        <v>44509.64800585648</v>
+        <v>44434.96418570602</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>745</v>
+        <v>767</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6">
-        <v>44511.67887549769</v>
+        <v>44497.47637053241</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>738</v>
+        <v>768</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6">
+        <v>44509.64800585648</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>746</v>
+      <c r="B33" s="2" t="s">
+        <v>770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2024-02-27 10:00:28 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
+++ b/_Drive/Formularios/Doutorado-FluxoContinuo/Inscrição para Doutorado (respostas).xlsx
@@ -593,12 +593,87 @@
         <t xml:space="preserve">Updated on 31-Oct-2023 07:11 PM</t>
       </text>
     </comment>
+    <comment authorId="0" ref="DT29">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:21 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU29">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:21 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV29">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:21 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW29">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:20 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX29">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:20 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DT30">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:55 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU30">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:55 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV30">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:55 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW30">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:55 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX30">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 10:55 AM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DT31">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 12:14 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DU31">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 12:14 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DV31">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 12:14 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DW31">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 12:14 PM</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="DX31">
+      <text>
+        <t xml:space="preserve">Updated on 26-Feb-2024 12:14 PM</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="836">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2822,19 +2897,214 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnuc7t411_eL6ysWa4cKfkru8dFWzjVg7XzuBbzvsn30d17uCDcpCv3T7eFcxDiBAj-0&amp;source=documentstudio&amp;timestamp=1698790269958</t>
   </si>
   <si>
+    <t>Vitória de Melo Silveira</t>
+  </si>
+  <si>
+    <t>vitoria.melo.silveira@usp.br</t>
+  </si>
+  <si>
+    <t>Atibaia</t>
+  </si>
+  <si>
+    <t>SP/Brasil</t>
+  </si>
+  <si>
+    <t>Rua Onofre Gemelli, 52</t>
+  </si>
+  <si>
+    <t>Nova Lorena</t>
+  </si>
+  <si>
+    <t>Anita Melo</t>
+  </si>
+  <si>
+    <t>Irmã</t>
+  </si>
+  <si>
+    <t>Rua Jasmin, 190, apto 54A</t>
+  </si>
+  <si>
+    <t>Chácara Primavera</t>
+  </si>
+  <si>
+    <t>Campinas</t>
+  </si>
+  <si>
+    <t>Escola de Engenharia de Lorena - Universidade de São Paulo</t>
+  </si>
+  <si>
+    <t>Engenheira de Materiais</t>
+  </si>
+  <si>
+    <t>Tenaris Confab</t>
+  </si>
+  <si>
+    <t>Estagiária de Qualidade-Consultas Técnicas</t>
+  </si>
+  <si>
+    <t>Estágio supervisionado em docência (PAE)</t>
+  </si>
+  <si>
+    <t>Busco me desenvolver academicamente estudando e colocando em prática meu projeto de pesquisa, além de cursar disciplinas que contribuam para meu conhecimento técnico sobre temas relacionados à minha área de pesquisa.</t>
+  </si>
+  <si>
+    <t>Determinação experimental de grandezas cinéticas nos sistemas Al-Ta, Al-Mo, Al-Nb e Al-Ta-Ti e modelagem de mobilidade na região CCC do sistema Al-Ta-Ti</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=19F4trcUPwABZE7pZpH-6LdaoAenOcU80</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IEQq55yHeXsH0JXUR76rorUw37vBUILV</t>
+  </si>
+  <si>
+    <t>53957-0</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IXEnDTN33Oxg8dORCMCdnMZXq_lrKwiW</t>
+  </si>
+  <si>
+    <t>2_ABaOnucmhepoqDQSmBRhNcjxJZhMw4lIhm4G-WE3MxllZPZEjxen3EIRJARk2BNR2lz6AdQ</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnucmhepoqDQSmBRhNcjxJZhMw4lIhm4G-WE3MxllZPZEjxen3EIRJARk2BNR2lz6AdQ&amp;source=documentstudio&amp;timestamp=1708953610310</t>
+  </si>
+  <si>
+    <t>Caio Simão de Barros</t>
+  </si>
+  <si>
+    <t>caio.simao.barros@usp.br</t>
+  </si>
+  <si>
+    <t>Av. Oswaldo Aranha, 919 - Ap. 21</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Rua Candido Diniz Junqueira, 7</t>
+  </si>
+  <si>
+    <t>Jardim Guapira</t>
+  </si>
+  <si>
+    <t>02316160</t>
+  </si>
+  <si>
+    <t>Gerdau Aços Especiais</t>
+  </si>
+  <si>
+    <t>Estagiário - Engenharia de Produto e Processo - Qualidade</t>
+  </si>
+  <si>
+    <t>Estagiário PAE</t>
+  </si>
+  <si>
+    <t>Poder continuar desenvolvendo trabalhos relacionados à pesquisa e ao ensino, assim como venho fazendo no mestrado.</t>
+  </si>
+  <si>
+    <t>Estudo experimental e modelagem termodinâmica do sistema Al-Nb-Ta</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1j5v5gAY-lN-YQjwSQbe3ZqDn9HrAeJfU</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1nA_6TFnwEOVTHnq9lYHyr3EFCNuZ4GEY</t>
+  </si>
+  <si>
+    <t>3571-8</t>
+  </si>
+  <si>
+    <t>26950-6</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17MXlx4SUT9j5Vqeby9zO6XJIyE0MeW08</t>
+  </si>
+  <si>
+    <t>2_ABaOnufJEYsJ_GuC0oV0QNJg-TXEJDKQ8fnIR2MpEJ4OTMZgADTFcGDosXMEu55f-2P9y94</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnufJEYsJ_GuC0oV0QNJg-TXEJDKQ8fnIR2MpEJ4OTMZgADTFcGDosXMEu55f-2P9y94&amp;source=documentstudio&amp;timestamp=1708955697862</t>
+  </si>
+  <si>
+    <t>Ana Carolina Brasil da Silva</t>
+  </si>
+  <si>
+    <t>anabrasil@usp.br</t>
+  </si>
+  <si>
+    <t>Rua Barão da Bocaina, 02</t>
+  </si>
+  <si>
+    <t>Ana Maria Brasil do Nascimento</t>
+  </si>
+  <si>
+    <t>Rua do Magistério, 86</t>
+  </si>
+  <si>
+    <t>Nova Angra</t>
+  </si>
+  <si>
+    <t>024999183965</t>
+  </si>
+  <si>
+    <t>Mestre/Engenharia de Materiais</t>
+  </si>
+  <si>
+    <t>Centro Federal de Educação Tecnológica Celso Suckow da Fonseca</t>
+  </si>
+  <si>
+    <t>Graduação/Engenharia Metalúrgica</t>
+  </si>
+  <si>
+    <t>Técnico/Técnico em Mecânica</t>
+  </si>
+  <si>
+    <t>Fazer meu doutorado em uma grande instituição e aperfeiçoar minha forma de fazer pesquisa.</t>
+  </si>
+  <si>
+    <t>Avaliação da influência da adição de Mo/Nb/Ta/Ti na oxidação de superligas à base de níquel para aplicações em discos de turbina através de investigação de ligas modelo 80Ni-18Cr-2M (%at. - M=Mo, Nb, Ta, Ti)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1x5GIjtmNA_x1iNP2hH3pv2f_OxxCCa-8</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1QIMPkn_sY0EB4g45gOvIr6cymM5RGQei</t>
+  </si>
+  <si>
+    <t>55014-0</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ud27Q4chMB-Ac9dfKwyPCplP0OsQ4Qt4</t>
+  </si>
+  <si>
+    <t>2_ABaOnucRpOMw0K0mTvfeiOwy8orqIzbf_Vw1wGlciAbpJG_92_3WPNa8YdEys9m3mt2wN68</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdcC8OxBYiJiDWMko1G13-gQfcteiPPgMJQaQNzpi9SQLUpvw/viewform?edit2=2_ABaOnucRpOMw0K0mTvfeiOwy8orqIzbf_Vw1wGlciAbpJG_92_3WPNa8YdEys9m3mt2wN68&amp;source=documentstudio&amp;timestamp=1708960424058</t>
+  </si>
+  <si>
     <t>Document Studio Logs</t>
   </si>
   <si>
     <t>👋🏻 Please do not edit or delete this sheet)</t>
   </si>
   <si>
+    <t>✔️  [Respostas] Processed form row #31 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #30 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>✔️  [Respostas] Processed form row #29 by luizeleno@usp.br</t>
+  </si>
+  <si>
+    <t>⚠️  Google Form has duplicate question titles</t>
+  </si>
+  <si>
+    <t>inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
+  </si>
+  <si>
     <t>✔️  [Respostas] Processed form row #28 by luizeleno@usp.br</t>
-  </si>
-  <si>
-    <t>⚠️  Google Form has duplicate question titles</t>
-  </si>
-  <si>
-    <t>inseriroutraexperiênciadeensino (Value changed from 'Sim' to 'Não')</t>
   </si>
   <si>
     <t>✔️  [Respostas] Processed form row #27 by luizeleno@usp.br</t>
@@ -10062,6 +10332,687 @@
         <v>739</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="6">
+        <v>45348.430674884265</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I29" s="7">
+        <v>35446.0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="L29" s="2">
+        <v>4.5578864856E10</v>
+      </c>
+      <c r="M29" s="2">
+        <v>4.58653214E8</v>
+      </c>
+      <c r="N29" s="7">
+        <v>43416.0</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P29" s="2">
+        <v>9359542.0</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T29" s="2">
+        <v>1.260256E7</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V29" s="2">
+        <v>1.1974624168E10</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="Z29" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="AA29" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="AC29" s="2">
+        <v>1.308746E7</v>
+      </c>
+      <c r="AD29" s="2">
+        <v>1.9987068243E10</v>
+      </c>
+      <c r="AE29" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="AF29" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AG29" s="7">
+        <v>45323.0</v>
+      </c>
+      <c r="AH29" s="7">
+        <v>45323.0</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ29" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="AK29" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="AL29" s="7">
+        <v>42036.0</v>
+      </c>
+      <c r="AM29" s="7">
+        <v>44581.0</v>
+      </c>
+      <c r="AN29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR29" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="BS29" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="BT29" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU29" s="7">
+        <v>44172.0</v>
+      </c>
+      <c r="BV29" s="7">
+        <v>44575.0</v>
+      </c>
+      <c r="BW29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP29" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="CQ29" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="CR29" s="7">
+        <v>44774.0</v>
+      </c>
+      <c r="CS29" s="7">
+        <v>44926.0</v>
+      </c>
+      <c r="CT29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU29" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="CV29" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="CW29" s="7">
+        <v>44958.0</v>
+      </c>
+      <c r="CX29" s="7">
+        <v>45107.0</v>
+      </c>
+      <c r="CY29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL29" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="DM29" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN29" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="DO29" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="DP29" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="DQ29" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR29" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="DS29" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="DT29" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="DU29" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1IXEnDTN33Oxg8dORCMCdnMZXq_lrKwiW","Inscrição DOUTORADO PPGEM EEL-USP - Vitória de Melo Silveira.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Vitória de Melo Silveira.pdf</v>
+      </c>
+      <c r="DV29" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18de594376b6cca8","Email sent to ppgem-eel@usp.br, vitoria.melo.silveira@usp.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, vitoria.melo.silveira@usp.br</v>
+      </c>
+      <c r="DW29" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="DX29" s="9" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6">
+        <v>45348.45483636574</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I30" s="7">
+        <v>35332.0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="L30" s="2">
+        <v>4.70040728E10</v>
+      </c>
+      <c r="M30" s="2">
+        <v>5.05787222E8</v>
+      </c>
+      <c r="N30" s="7">
+        <v>41988.0</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P30" s="2">
+        <v>8942235.0</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T30" s="2">
+        <v>1.2606E7</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V30" s="2">
+        <v>1.1971052265E10</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="Z30" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="AA30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC30" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="AD30" s="2">
+        <v>1.195732175E10</v>
+      </c>
+      <c r="AE30" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="AF30" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AG30" s="7">
+        <v>42044.0</v>
+      </c>
+      <c r="AH30" s="7">
+        <v>44582.0</v>
+      </c>
+      <c r="AI30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX30" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="AY30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BD30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BF30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BG30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR30" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="BS30" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="BT30" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BU30" s="7">
+        <v>44228.0</v>
+      </c>
+      <c r="BV30" s="7">
+        <v>44547.0</v>
+      </c>
+      <c r="BW30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CP30" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="CQ30" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="CR30" s="7">
+        <v>44774.0</v>
+      </c>
+      <c r="CS30" s="7">
+        <v>44926.0</v>
+      </c>
+      <c r="CT30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU30" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="CV30" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="CW30" s="7">
+        <v>44958.0</v>
+      </c>
+      <c r="CX30" s="7">
+        <v>45107.0</v>
+      </c>
+      <c r="CY30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL30" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="DM30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN30" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="DO30" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="DP30" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="DQ30" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR30" s="8" t="s">
+        <v>778</v>
+      </c>
+      <c r="DS30" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="DT30" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="DU30" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=17MXlx4SUT9j5Vqeby9zO6XJIyE0MeW08","Inscrição DOUTORADO PPGEM EEL-USP - Caio Simão de Barros.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Caio Simão de Barros.pdf</v>
+      </c>
+      <c r="DV30" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18de5b307ec83c0f","Email sent to ppgem-eel@usp.br, caio.simao.barros@usp.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, caio.simao.barros@usp.br</v>
+      </c>
+      <c r="DW30" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="DX30" s="9" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6">
+        <v>45348.509537708334</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="7">
+        <v>34935.0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1.6103921759E10</v>
+      </c>
+      <c r="M31" s="2">
+        <v>2.89669467E8</v>
+      </c>
+      <c r="N31" s="7">
+        <v>41628.0</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1.3556853E7</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T31" s="2">
+        <v>1.260023E7</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V31" s="2">
+        <v>2.4999889835E10</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB31" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC31" s="2">
+        <v>2.3933295E7</v>
+      </c>
+      <c r="AD31" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="AE31" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="AF31" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="AG31" s="7">
+        <v>44593.0</v>
+      </c>
+      <c r="AH31" s="7">
+        <v>45383.0</v>
+      </c>
+      <c r="AI31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ31" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="AK31" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="AL31" s="7">
+        <v>42038.0</v>
+      </c>
+      <c r="AM31" s="7">
+        <v>44587.0</v>
+      </c>
+      <c r="AN31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO31" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="AP31" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="AQ31" s="7">
+        <v>40575.0</v>
+      </c>
+      <c r="AR31" s="7">
+        <v>41993.0</v>
+      </c>
+      <c r="AS31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AZ31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BB31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BQ31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CO31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DI31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DL31" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="DM31" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DN31" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="DO31" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="DP31" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="DQ31" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="DR31" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="DS31" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="DT31" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="DU31" s="11" t="str">
+        <f>HYPERLINK("https://drive.google.com/open?id=1ud27Q4chMB-Ac9dfKwyPCplP0OsQ4Qt4","Inscrição DOUTORADO PPGEM EEL-USP - Ana Carolina Brasil da Silva.pdf")</f>
+        <v>Inscrição DOUTORADO PPGEM EEL-USP - Ana Carolina Brasil da Silva.pdf</v>
+      </c>
+      <c r="DV31" s="11" t="str">
+        <f>HYPERLINK("https://mail.google.com/mail/u/0/#all/18de5fb65a784943","Email sent to ppgem-eel@usp.br, anabrasil@usp.br")</f>
+        <v>Email sent to ppgem-eel@usp.br, anabrasil@usp.br</v>
+      </c>
+      <c r="DW31" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="DX31" s="9" t="s">
+        <v>801</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="DO2"/>
@@ -10161,9 +11112,21 @@
     <hyperlink r:id="rId96" ref="DP28"/>
     <hyperlink r:id="rId97" ref="DT28"/>
     <hyperlink r:id="rId98" ref="DX28"/>
+    <hyperlink r:id="rId99" ref="DO29"/>
+    <hyperlink r:id="rId100" ref="DP29"/>
+    <hyperlink r:id="rId101" ref="DT29"/>
+    <hyperlink r:id="rId102" ref="DX29"/>
+    <hyperlink r:id="rId103" ref="DO30"/>
+    <hyperlink r:id="rId104" ref="DP30"/>
+    <hyperlink r:id="rId105" ref="DT30"/>
+    <hyperlink r:id="rId106" ref="DX30"/>
+    <hyperlink r:id="rId107" ref="DO31"/>
+    <hyperlink r:id="rId108" ref="DP31"/>
+    <hyperlink r:id="rId109" ref="DT31"/>
+    <hyperlink r:id="rId110" ref="DX31"/>
   </hyperlinks>
-  <drawing r:id="rId99"/>
-  <legacyDrawing r:id="rId100"/>
+  <drawing r:id="rId111"/>
+  <legacyDrawing r:id="rId112"/>
 </worksheet>
 </file>
 
@@ -10182,320 +11145,358 @@
         <v>44376.74002457176</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>740</v>
+        <v>802</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>741</v>
+        <v>803</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>45230.80012315972</v>
+        <v>45348.51015188657</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>742</v>
+        <v>804</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="6">
-        <v>45230.79985361111</v>
+        <v>45348.45524628472</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>744</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="6">
-        <v>45229.75742496528</v>
+        <v>45348.431874965274</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>745</v>
+        <v>806</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="6">
-        <v>45229.75720832176</v>
+        <v>45348.43099300926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>746</v>
+        <v>808</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6">
-        <v>45229.43523862268</v>
+        <v>45230.80012315972</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>747</v>
+        <v>809</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="6">
-        <v>45229.434958645834</v>
+        <v>45230.79985361111</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>746</v>
+        <v>808</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6">
-        <v>45078.61406284722</v>
+        <v>45229.75742496528</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>748</v>
+        <v>810</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="6">
-        <v>45071.65914045139</v>
+        <v>45229.75720832176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>807</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6">
-        <v>45071.658906192126</v>
+        <v>45229.43523862268</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>750</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
-        <v>44867.38816256945</v>
+        <v>45229.434958645834</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>807</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6">
-        <v>44853.70966662037</v>
+        <v>45078.61406284722</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>752</v>
+        <v>813</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="6">
-        <v>44853.694473275464</v>
+        <v>45071.65914045139</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>753</v>
+        <v>814</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="6">
-        <v>44853.69422237268</v>
+        <v>45071.658906192126</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>746</v>
+        <v>815</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6">
-        <v>44830.76710104167</v>
+        <v>44867.38816256945</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>754</v>
+        <v>816</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="6">
-        <v>44784.87304421296</v>
+        <v>44853.70966662037</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>755</v>
+        <v>817</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="6">
-        <v>44784.87274673611</v>
+        <v>44853.694473275464</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>744</v>
-      </c>
+        <v>818</v>
+      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="6">
-        <v>44770.501262986116</v>
+        <v>44853.69422237268</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>807</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6">
-        <v>44757.68569034722</v>
+        <v>44830.76710104167</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>757</v>
+        <v>819</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="6">
-        <v>44756.72330104167</v>
+        <v>44784.87304421296</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>758</v>
+        <v>820</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="6">
-        <v>44649.34401880787</v>
+        <v>44784.87274673611</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>807</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="6">
-        <v>44649.343747569445</v>
+        <v>44770.501262986116</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>760</v>
-      </c>
+        <v>821</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="6">
-        <v>44648.7586062037</v>
+        <v>44757.68569034722</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>761</v>
+        <v>822</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="6">
-        <v>44648.75839336806</v>
+        <v>44756.72330104167</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>762</v>
-      </c>
+        <v>823</v>
+      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="6">
-        <v>44376.74045414352</v>
+        <v>44649.34401880787</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>763</v>
-      </c>
+        <v>824</v>
+      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="6">
-        <v>44400.52960546296</v>
+        <v>44649.343747569445</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>762</v>
+        <v>825</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6">
-        <v>44400.5298077662</v>
+        <v>44648.7586062037</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>765</v>
-      </c>
+        <v>826</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="6">
-        <v>44434.96399693287</v>
+        <v>44648.75839336806</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>766</v>
+        <v>827</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6">
-        <v>44434.96418570602</v>
+        <v>44376.74045414352</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>765</v>
+        <v>828</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6">
-        <v>44497.47637053241</v>
+        <v>44400.52960546296</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>768</v>
+        <v>807</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6">
-        <v>44509.64800585648</v>
+        <v>44400.5298077662</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>769</v>
+        <v>829</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6">
-        <v>44511.67887549769</v>
+        <v>44434.96399693287</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>743</v>
+        <v>807</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>762</v>
+        <v>831</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6">
+        <v>44434.96418570602</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6">
+        <v>44497.47637053241</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6">
+        <v>44509.64800585648</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6">
+        <v>44511.67887549769</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6">
         <v>44511.67908989583</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>770</v>
+      <c r="B37" s="2" t="s">
+        <v>835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>